<commit_message>
Added 2nd Test Case and validated the Username in 1st Test case
</commit_message>
<xml_diff>
--- a/src/test/TestData/Test Cases.xlsx
+++ b/src/test/TestData/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareTesting\Workspaces\RealTimeProject\Automation_Framework_E-Commerce\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDBE93D-0464-44BF-8F44-71E2656E11B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05AB4E1-DED1-4CD4-941A-C444997AFA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Comments</t>
   </si>
   <si>
     <t>Requirement Screen/Module</t>
@@ -93,24 +90,9 @@
     <t>Verify User Login functionality</t>
   </si>
   <si>
-    <t>1. Launch Browser
-2. Open the URL
-3. Click on Sign in link on Homepage
-4. Enter Username and Password in Login Page
-5. Click on Sign In button
-6. Validate that the Actual User has logged in Dashboard</t>
-  </si>
-  <si>
     <t>https://magento.softwaretestingboard.com/
 Username-
 Password-</t>
-  </si>
-  <si>
-    <t>1. Portal should be launch and URL should be working
-2. Homepage should be displayed with Sign In link
-3. Login Page should be displayed with textbox for Username and password with Sign in button
-4. User should be loggen in with Valid credentials
-5. On Dashbaord page- username should be displayed</t>
   </si>
   <si>
     <t>TC002</t>
@@ -122,6 +104,52 @@
 4. Enter First Name, Last Name, Email, Password and Confirm Password
 5. Click on Create an Account
 6. On the Dashboard-Validate that the User Account is Created</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Dashboard Page</t>
+  </si>
+  <si>
+    <t>User Account Credentials should be available</t>
+  </si>
+  <si>
+    <t>Execution Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Verify Dashbaord Page functional componets</t>
+  </si>
+  <si>
+    <t>1. Launch Browser
+2. Open the URL
+3. Click on Sign in link on Homepage
+4. Enter Username and Password in Login Page
+5. Click on Sign In button
+6. Validate the Logged In Username</t>
+  </si>
+  <si>
+    <t>1. Launch Browser
+2. Open the URL
+3. Click on Sign in link on Homepage
+4. Enter Username and Password in Login Page
+5. Click on Sign In button</t>
+  </si>
+  <si>
+    <t>1. Portal should be launch and URL should be working
+2. Homepage should be displayed with Sign In link
+3. Login Page should be displayed with textbox for Username and password with Sign in button
+4. User should be loggen in with Valid credentials</t>
+  </si>
+  <si>
+    <t>1. On Dashbaord page- Logged In Username should be displayed
+2. Username should be matching with Profile with actual User</t>
   </si>
 </sst>
 </file>
@@ -235,7 +263,307 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -565,21 +893,22 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="2"/>
-    <col min="9" max="9" width="22.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="4.88671875" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="3.21875" style="1" customWidth="1"/>
@@ -591,10 +920,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1</v>
@@ -615,76 +944,98 @@
         <v>6</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="D4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="J4" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -696,7 +1047,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
@@ -708,7 +1059,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="7"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -720,7 +1071,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="7"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -732,7 +1083,7 @@
       <c r="G8" s="8"/>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
@@ -744,7 +1095,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
@@ -756,7 +1107,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
@@ -768,7 +1119,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
@@ -780,7 +1131,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
@@ -792,7 +1143,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
@@ -804,7 +1155,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
@@ -816,7 +1167,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="7"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
@@ -828,109 +1179,145 @@
       <c r="G16" s="8"/>
       <c r="H16" s="7"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H2:H3">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+  <conditionalFormatting sqref="H2:H4">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{362524A8-7438-44BF-A0CA-A18DD8F36D9A}">
+  <conditionalFormatting sqref="J2:J4">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Untested"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Not Applicable"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4" xr:uid="{362524A8-7438-44BF-A0CA-A18DD8F36D9A}">
       <formula1>"Critical, High, Medium, Low"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{F08AC2E7-1D15-473A-BD5D-4FA8D9137F99}">
+      <formula1>"Pass, Fail, Untested, Not Applicable"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{6E439BD3-5AE5-4B4F-A36E-A6A9A65FDCE0}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{D8B53542-FFD0-4186-996A-A49010C90664}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{1B769CB6-950F-4B6F-AE9D-4F5E0E48D2AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented Screenshots to be taken for Failed Test Cases and Extent Report with New Test Case
</commit_message>
<xml_diff>
--- a/src/test/TestData/Test Cases.xlsx
+++ b/src/test/TestData/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareTesting\Workspaces\RealTimeProject\Automation_Framework_E-Commerce\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05AB4E1-DED1-4CD4-941A-C444997AFA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989F1DDF-0383-42FA-926D-81191F9AD444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,21 +135,23 @@
 6. Validate the Logged In Username</t>
   </si>
   <si>
+    <t>1. On Dashbaord page- Logged In Username should be displayed
+2. Username should be matching with Profile with actual User</t>
+  </si>
+  <si>
+    <t>1. Portal should be launch and URL should be working
+2. Homepage should be displayed with Sign In link
+3. Login Page should be displayed with textbox for Username and password with Sign in button
+4. User should be loggen in with Valid credentials
+5. Username should be dispplayed</t>
+  </si>
+  <si>
     <t>1. Launch Browser
 2. Open the URL
 3. Click on Sign in link on Homepage
-4. Enter Username and Password in Login Page
-5. Click on Sign In button</t>
-  </si>
-  <si>
-    <t>1. Portal should be launch and URL should be working
-2. Homepage should be displayed with Sign In link
-3. Login Page should be displayed with textbox for Username and password with Sign in button
-4. User should be loggen in with Valid credentials</t>
-  </si>
-  <si>
-    <t>1. On Dashbaord page- Logged In Username should be displayed
-2. Username should be matching with Profile with actual User</t>
+4. Enter Valid Username and Valid Password in Login Page
+5. Click on Sign In button
+6. Verify Logged in Username is visible on webpage</t>
   </si>
 </sst>
 </file>
@@ -263,7 +265,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -301,266 +303,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0070C0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -893,7 +635,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -977,7 +719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
@@ -991,7 +733,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>20</v>
@@ -1027,7 +769,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>12</v>
@@ -1276,34 +1018,34 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H2:H4">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J4">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"Pass"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Not Applicable"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Untested"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Untested"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Not Applicable"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Resolving Errors for test cases
</commit_message>
<xml_diff>
--- a/src/test/TestData/Test Cases.xlsx
+++ b/src/test/TestData/Test Cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareTesting\Workspaces\RealTimeProject\Automation_Framework_E-Commerce\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989F1DDF-0383-42FA-926D-81191F9AD444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D71AD-30D8-4DD4-90F2-C0B7BDA31800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -152,6 +152,9 @@
 4. Enter Valid Username and Valid Password in Login Page
 5. Click on Sign In button
 6. Verify Logged in Username is visible on webpage</t>
+  </si>
+  <si>
+    <t>Working as per expected</t>
   </si>
 </sst>
 </file>
@@ -634,9 +637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -714,7 +717,9 @@
       <c r="H2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="J2" s="7" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Implemented Email Generator to pick the uniques Email everytime to Create the Account for TC001
</commit_message>
<xml_diff>
--- a/src/test/TestData/Test Cases.xlsx
+++ b/src/test/TestData/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareTesting\Workspaces\RealTimeProject\Automation_Framework_E-Commerce\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D71AD-30D8-4DD4-90F2-C0B7BDA31800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90148FBB-1E72-4CB9-9A06-DE5E7A9911A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -88,11 +88,6 @@
   </si>
   <si>
     <t>Verify User Login functionality</t>
-  </si>
-  <si>
-    <t>https://magento.softwaretestingboard.com/
-Username-
-Password-</t>
   </si>
   <si>
     <t>TC002</t>
@@ -121,9 +116,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>Verify Dashbaord Page functional componets</t>
   </si>
   <si>
@@ -156,12 +148,17 @@
   <si>
     <t>Working as per expected</t>
   </si>
+  <si>
+    <t>https://magento.softwaretestingboard.com/
+Username
+Password</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,14 +170,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,11 +219,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -260,12 +248,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -639,7 +629,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,7 +639,7 @@
     <col min="3" max="3" width="18.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" style="4" customWidth="1"/>
     <col min="7" max="7" width="33.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
@@ -689,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
@@ -706,9 +696,9 @@
         <v>16</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -718,15 +708,15 @@
         <v>11</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>14</v>
@@ -738,51 +728,51 @@
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="G3" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="J3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="8"/>
-      <c r="J4" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1018,10 +1008,14 @@
       <c r="H34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="4"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Medium"</formula>
@@ -1061,11 +1055,6 @@
       <formula1>"Pass, Fail, Untested, Not Applicable"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{6E439BD3-5AE5-4B4F-A36E-A6A9A65FDCE0}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{D8B53542-FFD0-4186-996A-A49010C90664}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{1B769CB6-950F-4B6F-AE9D-4F5E0E48D2AD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented Test Case -05 for Dashboard Page and also implemented fetching the user credentials from properties file globally using custom methods
</commit_message>
<xml_diff>
--- a/src/test/TestData/Test Cases.xlsx
+++ b/src/test/TestData/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareTesting\Workspaces\RealTimeProject\Automation_Framework_E-Commerce\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90148FBB-1E72-4CB9-9A06-DE5E7A9911A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8373DE59-3651-4EFF-8428-725D842E18B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -119,18 +119,6 @@
     <t>Verify Dashbaord Page functional componets</t>
   </si>
   <si>
-    <t>1. Launch Browser
-2. Open the URL
-3. Click on Sign in link on Homepage
-4. Enter Username and Password in Login Page
-5. Click on Sign In button
-6. Validate the Logged In Username</t>
-  </si>
-  <si>
-    <t>1. On Dashbaord page- Logged In Username should be displayed
-2. Username should be matching with Profile with actual User</t>
-  </si>
-  <si>
     <t>1. Portal should be launch and URL should be working
 2. Homepage should be displayed with Sign In link
 3. Login Page should be displayed with textbox for Username and password with Sign in button
@@ -152,6 +140,34 @@
     <t>https://magento.softwaretestingboard.com/
 Username
 Password</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Verify the Create Account- User Registration Functionality with Data Driven concept</t>
+  </si>
+  <si>
+    <t>Verify User Login functionality with Data Driven concept</t>
+  </si>
+  <si>
+    <t>1. Launch Browser
+2. Open the URL
+3. Click on Sign in link on Homepage
+4. Enter Username and Password in Login Page
+5. Click on Sign In button
+6. Go to Dashboard and validate following functionality-
+-LUMA logo link
+-Page Title
+-Navigation links- Whats new
+-Women-</t>
+  </si>
+  <si>
+    <t>Store Logo link should be working
+-Page title should be correct</t>
   </si>
 </sst>
 </file>
@@ -222,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,12 +262,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -625,11 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +708,7 @@
       <c r="E2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -708,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>26</v>
@@ -728,73 +738,113 @@
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="4" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="E6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="7"/>
       <c r="I6" s="8"/>
       <c r="J6" s="7"/>
     </row>
@@ -919,14 +969,28 @@
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
@@ -1008,15 +1072,25 @@
       <c r="H34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="4"/>
+    <row r="35" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
@@ -1033,7 +1107,7 @@
       <formula>"Critical"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Not Applicable"</formula>
     </cfRule>
@@ -1048,10 +1122,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4" xr:uid="{362524A8-7438-44BF-A0CA-A18DD8F36D9A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6" xr:uid="{362524A8-7438-44BF-A0CA-A18DD8F36D9A}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{F08AC2E7-1D15-473A-BD5D-4FA8D9137F99}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6" xr:uid="{F08AC2E7-1D15-473A-BD5D-4FA8D9137F99}">
       <formula1>"Pass, Fail, Untested, Not Applicable"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added Test case-6 to search a product and get the name of the product
</commit_message>
<xml_diff>
--- a/src/test/TestData/Test Cases.xlsx
+++ b/src/test/TestData/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareTesting\Workspaces\RealTimeProject\Automation_Framework_E-Commerce\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8373DE59-3651-4EFF-8428-725D842E18B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0C43B-56B1-48C8-8343-1341DC4F7375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -168,6 +168,32 @@
   <si>
     <t>Store Logo link should be working
 -Page title should be correct</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>Dashboard Page&gt;&gt;Search Product</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>1. Launch Browser
+2. Open the URL
+3. Click on Sign in link on Homepage
+4. Enter Username and Password in Login Page
+5. Click on Sign In button
+6. Go to Dashboard and click on Search textbox
+7. Enter product name- Jackets in search box and click on search icon
+8. Validate the search result displayed and Jackets product displays
+9. click on Sign out</t>
+  </si>
+  <si>
+    <t>Jacket product should be displayed</t>
+  </si>
+  <si>
+    <t>Verify the Search product functionality on the Dashboard Page</t>
   </si>
 </sst>
 </file>
@@ -638,8 +664,8 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,15 +874,31 @@
       <c r="I6" s="8"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="7"/>
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="7"/>
     </row>
@@ -1090,7 +1132,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
@@ -1122,7 +1164,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6" xr:uid="{362524A8-7438-44BF-A0CA-A18DD8F36D9A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{362524A8-7438-44BF-A0CA-A18DD8F36D9A}">
       <formula1>"Critical, High, Medium, Low"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6" xr:uid="{F08AC2E7-1D15-473A-BD5D-4FA8D9137F99}">

</xml_diff>